<commit_message>
Renamed arcs to links
</commit_message>
<xml_diff>
--- a/tests/test_case1.xlsx
+++ b/tests/test_case1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srs\source\repos\snra\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srs\src\snram\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="2" r:id="rId1"/>
-    <sheet name="arcs" sheetId="1" r:id="rId2"/>
+    <sheet name="links" sheetId="1" r:id="rId2"/>
     <sheet name="scale" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -421,38 +421,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -466,18 +466,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -519,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -547,7 +547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -575,19 +575,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -607,17 +607,17 @@
       <selection activeCell="C9" sqref="C9:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -625,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -633,7 +633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -641,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -649,7 +649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -657,12 +657,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -670,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>5</v>
       </c>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -694,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>14</v>
       </c>

</xml_diff>